<commit_message>
ajout des dépenses d'hier soir
</commit_message>
<xml_diff>
--- a/Other files/Dépenses.xlsx
+++ b/Other files/Dépenses.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie-France\Documents\GitHub\Majabaja\Other files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="72" windowWidth="22116" windowHeight="10080"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Dépenses reliées à la GCA</t>
   </si>
@@ -40,6 +45,12 @@
   </si>
   <si>
     <t>Notes additionnels</t>
+  </si>
+  <si>
+    <t>Marie-France Miousse</t>
+  </si>
+  <si>
+    <t>Lait + jambon</t>
   </si>
 </sst>
 </file>
@@ -108,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -121,6 +132,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -131,12 +143,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -178,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,7 +228,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,26 +440,26 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -461,7 +476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>41654</v>
       </c>
@@ -476,42 +491,52 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>41655</v>
+      </c>
+      <c r="B6" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7">
+        <v>126.29</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="7"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="7"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="7"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="7"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -530,7 +555,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -542,7 +567,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>